<commit_message>
GI05MOAS GL484 Ingest CSV
Created Ingest CSV for GL484 D2
</commit_message>
<xml_diff>
--- a/GI05MOAS-GL484/Omaha_Cal_Info_GI05MOAS-GL484_00002.xlsx
+++ b/GI05MOAS-GL484/Omaha_Cal_Info_GI05MOAS-GL484_00002.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\GI05MOAS-GL484\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="800" windowWidth="25520" windowHeight="11040" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="9915" yWindow="795" windowWidth="25515" windowHeight="11040" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$99</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$379</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -103,18 +108,6 @@
   </si>
   <si>
     <t>CC_depolarization_ratio</t>
-  </si>
-  <si>
-    <t>GI05MOAS-GL001-01-FLORDM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-GL001-02-DOSTAM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-GL001-04-CTDGVM000</t>
-  </si>
-  <si>
-    <t>GI05MOAS-GL001-00-ENG000000</t>
   </si>
   <si>
     <t>FLBBSLC-3550</t>
@@ -158,6 +151,18 @@
       </rPr>
       <t>30-01</t>
     </r>
+  </si>
+  <si>
+    <t>GI05MOAS-GL484-01-FLORDM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-GL484-02-DOSTAM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-GL484-04-CTDGVM000</t>
+  </si>
+  <si>
+    <t>GI05MOAS-GL484-00-ENG000000</t>
   </si>
 </sst>
 </file>
@@ -595,6 +600,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -890,19 +898,19 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="21" customWidth="1"/>
     <col min="9" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,9 +945,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="15">
+    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="23">
         <v>484</v>
@@ -957,16 +965,16 @@
         <v>42243</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I2" s="23">
         <v>1000</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="21">
@@ -994,21 +1002,21 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1028,9 +1036,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B2" s="11">
         <v>484</v>
@@ -1039,7 +1047,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>16</v>
@@ -1051,9 +1059,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B3" s="20">
         <v>484</v>
@@ -1062,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>18</v>
@@ -1074,9 +1082,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B4" s="20">
         <v>484</v>
@@ -1085,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>19</v>
@@ -1097,9 +1105,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B5" s="20">
         <v>484</v>
@@ -1108,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>20</v>
@@ -1120,7 +1128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1">
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="19"/>
       <c r="C6" s="11"/>
@@ -1134,9 +1142,9 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1">
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="19">
         <v>484</v>
@@ -1158,7 +1166,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="19"/>
       <c r="C8" s="11"/>
@@ -1172,9 +1180,9 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" s="19">
         <v>484</v>
@@ -1196,7 +1204,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="19"/>
       <c r="C10" s="11"/>
@@ -1210,9 +1218,9 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1">
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B11" s="19">
         <v>484</v>
@@ -1234,7 +1242,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1">
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>

</xml_diff>